<commit_message>
calculated lipid titre values
</commit_message>
<xml_diff>
--- a/data/Data_F1.xlsx
+++ b/data/Data_F1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/pra100_csiro_au/Documents/Documents/Lipids_manuscript02/Updated Tables and Figures 130824/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/pra100_csiro_au/Documents/Documents/Lipids_manuscript02/Qfly_domestication/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="8_{A1D12656-BE65-4D83-8667-FBA7005B926B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{600D0E97-1365-49B9-8AF3-C1E5546FFCCC}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="8_{A1D12656-BE65-4D83-8667-FBA7005B926B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9FAE138-471A-4F8C-A7C1-4A291431DD12}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E200BEC2-E4DD-47C8-9E02-F4549D1DECE6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E200BEC2-E4DD-47C8-9E02-F4549D1DECE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -239,37 +239,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,55 +598,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3582FE2B-FBA7-477D-9390-AEEE4D7CC41D}">
   <dimension ref="A1:AP16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -664,126 +655,126 @@
       <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AD1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AE1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AF1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AG1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AH1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AI1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AJ1" s="7" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AK1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AL1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AM1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AN1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AO1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AP1" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1">
@@ -792,25 +783,25 @@
       <c r="D2" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E2" s="1">
-        <v>1782</v>
-      </c>
-      <c r="F2" s="1">
-        <v>67</v>
+      <c r="E2" s="7">
+        <v>0.19</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.01</v>
       </c>
       <c r="G2" s="1">
         <v>212</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>39.79</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>2.2999999999999998</v>
       </c>
       <c r="J2" s="1">
         <v>124</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="3">
         <v>54.53</v>
       </c>
       <c r="L2" s="1">
@@ -819,99 +810,99 @@
       <c r="M2" s="1">
         <v>16</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <v>1.39</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="2">
         <v>0.05</v>
       </c>
       <c r="P2" s="1">
         <v>21</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="3">
         <v>4.29</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="2">
         <v>0.22</v>
       </c>
       <c r="S2" s="1">
         <v>16.399999999999999</v>
       </c>
-      <c r="T2" s="7">
+      <c r="T2" s="2">
         <v>0.05</v>
       </c>
       <c r="U2" s="1">
         <v>17.46</v>
       </c>
-      <c r="V2" s="7">
+      <c r="V2" s="2">
         <v>0.01</v>
       </c>
       <c r="W2" s="1">
         <v>19.18</v>
       </c>
-      <c r="X2" s="5">
+      <c r="X2" s="2">
         <v>0.24</v>
       </c>
       <c r="Y2" s="1">
         <v>17.16</v>
       </c>
-      <c r="Z2" s="5">
+      <c r="Z2" s="2">
         <v>0.14000000000000001</v>
       </c>
       <c r="AA2" s="1">
         <v>14.16</v>
       </c>
-      <c r="AB2" s="5">
+      <c r="AB2" s="2">
         <v>0.02</v>
       </c>
       <c r="AC2" s="1">
         <v>22.08</v>
       </c>
-      <c r="AD2" s="5">
+      <c r="AD2" s="2">
         <v>0.02</v>
       </c>
       <c r="AE2" s="1">
         <v>0.91</v>
       </c>
-      <c r="AF2" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="AG2" s="3">
+      <c r="AF2" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="AG2" s="1">
         <v>1.47</v>
       </c>
-      <c r="AH2" s="7">
+      <c r="AH2" s="2">
         <v>0.01</v>
       </c>
       <c r="AI2" s="1">
         <v>0.05</v>
       </c>
-      <c r="AJ2" s="5">
+      <c r="AJ2" s="2">
         <v>0.04</v>
       </c>
       <c r="AK2" s="1">
         <v>0.9</v>
       </c>
-      <c r="AL2" s="5">
+      <c r="AL2" s="2">
         <v>0.04</v>
       </c>
-      <c r="AM2" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="AN2" s="7">
+      <c r="AM2" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="AN2" s="2">
         <v>0</v>
       </c>
       <c r="AO2" s="1">
         <v>1.81</v>
       </c>
-      <c r="AP2" s="7">
+      <c r="AP2" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1">
@@ -920,25 +911,25 @@
       <c r="D3" s="1">
         <v>0.33</v>
       </c>
-      <c r="E3" s="1">
-        <v>1708</v>
-      </c>
-      <c r="F3" s="1">
-        <v>87</v>
+      <c r="E3" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.02</v>
       </c>
       <c r="G3" s="1">
         <v>190</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>21.85</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>2.2400000000000002</v>
       </c>
       <c r="J3" s="1">
         <v>154</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>73.31</v>
       </c>
       <c r="L3" s="1">
@@ -947,99 +938,99 @@
       <c r="M3" s="1">
         <v>16</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>0.56000000000000005</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="2">
         <v>0.13</v>
       </c>
       <c r="P3" s="1">
         <v>17</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3" s="3">
         <v>4.28</v>
       </c>
-      <c r="R3" s="5">
+      <c r="R3" s="2">
         <v>0.18</v>
       </c>
       <c r="S3" s="1">
         <v>16.440000000000001</v>
       </c>
-      <c r="T3" s="7">
+      <c r="T3" s="2">
         <v>0.11</v>
       </c>
       <c r="U3" s="1">
         <v>17.29</v>
       </c>
-      <c r="V3" s="7">
+      <c r="V3" s="2">
         <v>0.04</v>
       </c>
       <c r="W3" s="1">
         <v>18.96</v>
       </c>
-      <c r="X3" s="5">
+      <c r="X3" s="2">
         <v>0.22</v>
       </c>
       <c r="Y3" s="1">
         <v>17.53</v>
       </c>
-      <c r="Z3" s="5">
+      <c r="Z3" s="2">
         <v>0.15</v>
       </c>
       <c r="AA3" s="1">
         <v>13.94</v>
       </c>
-      <c r="AB3" s="5">
+      <c r="AB3" s="2">
         <v>0.06</v>
       </c>
       <c r="AC3" s="1">
         <v>21.98</v>
       </c>
-      <c r="AD3" s="5">
+      <c r="AD3" s="2">
         <v>0.05</v>
       </c>
       <c r="AE3" s="1">
         <v>0.61</v>
       </c>
-      <c r="AF3" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="AG3" s="3">
+      <c r="AF3" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="AG3" s="1">
         <v>1.21</v>
       </c>
-      <c r="AH3" s="7">
+      <c r="AH3" s="2">
         <v>0.03</v>
       </c>
       <c r="AI3" s="1">
         <v>0.73</v>
       </c>
-      <c r="AJ3" s="5">
+      <c r="AJ3" s="2">
         <v>0.24</v>
       </c>
       <c r="AK3" s="1">
         <v>0.63</v>
       </c>
-      <c r="AL3" s="5">
+      <c r="AL3" s="2">
         <v>0.09</v>
       </c>
-      <c r="AM3" s="3">
+      <c r="AM3" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN3" s="7">
+      <c r="AN3" s="2">
         <v>0</v>
       </c>
       <c r="AO3" s="1">
         <v>1.27</v>
       </c>
-      <c r="AP3" s="7">
+      <c r="AP3" s="2">
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1">
@@ -1048,25 +1039,25 @@
       <c r="D4" s="1">
         <v>0.1</v>
       </c>
-      <c r="E4" s="1">
-        <v>1541</v>
-      </c>
-      <c r="F4" s="1">
-        <v>57</v>
+      <c r="E4" s="7">
+        <v>0.13</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.01</v>
       </c>
       <c r="G4" s="1">
         <v>209</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>27.17</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>2.04</v>
       </c>
       <c r="J4" s="1">
         <v>127</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>65.83</v>
       </c>
       <c r="L4" s="1">
@@ -1075,99 +1066,99 @@
       <c r="M4" s="1">
         <v>16</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>1.38</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="2">
         <v>0.05</v>
       </c>
       <c r="P4" s="1">
         <v>20</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <v>5.61</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="2">
         <v>0.28999999999999998</v>
       </c>
       <c r="S4" s="1">
         <v>16.39</v>
       </c>
-      <c r="T4" s="7">
+      <c r="T4" s="2">
         <v>0.06</v>
       </c>
       <c r="U4" s="1">
         <v>17.39</v>
       </c>
-      <c r="V4" s="7">
+      <c r="V4" s="2">
         <v>0.02</v>
       </c>
       <c r="W4" s="1">
         <v>19.28</v>
       </c>
-      <c r="X4" s="5">
+      <c r="X4" s="2">
         <v>0.26</v>
       </c>
       <c r="Y4" s="1">
         <v>17.32</v>
       </c>
-      <c r="Z4" s="5">
+      <c r="Z4" s="2">
         <v>0.16</v>
       </c>
       <c r="AA4" s="1">
         <v>14.15</v>
       </c>
-      <c r="AB4" s="5">
+      <c r="AB4" s="2">
         <v>0.03</v>
       </c>
       <c r="AC4" s="1">
         <v>22.07</v>
       </c>
-      <c r="AD4" s="5">
+      <c r="AD4" s="2">
         <v>0.04</v>
       </c>
       <c r="AE4" s="1">
         <v>0.89</v>
       </c>
-      <c r="AF4" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="AG4" s="3">
+      <c r="AF4" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="AG4" s="1">
         <v>1.4</v>
       </c>
-      <c r="AH4" s="7">
+      <c r="AH4" s="2">
         <v>0.03</v>
       </c>
       <c r="AI4" s="1">
         <v>0.06</v>
       </c>
-      <c r="AJ4" s="5">
+      <c r="AJ4" s="2">
         <v>0.03</v>
       </c>
       <c r="AK4" s="1">
         <v>0.94</v>
       </c>
-      <c r="AL4" s="5">
+      <c r="AL4" s="2">
         <v>0.06</v>
       </c>
-      <c r="AM4" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="AN4" s="7">
+      <c r="AM4" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="AN4" s="2">
         <v>0</v>
       </c>
       <c r="AO4" s="1">
         <v>1.75</v>
       </c>
-      <c r="AP4" s="7">
+      <c r="AP4" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1">
@@ -1176,25 +1167,25 @@
       <c r="D5" s="1">
         <v>0.23</v>
       </c>
-      <c r="E5" s="1">
-        <v>1935</v>
-      </c>
-      <c r="F5" s="1">
-        <v>85</v>
+      <c r="E5" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.02</v>
       </c>
       <c r="G5" s="1">
         <v>199</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>24.51</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>2.02</v>
       </c>
       <c r="J5" s="1">
         <v>151</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>70.91</v>
       </c>
       <c r="L5" s="1">
@@ -1203,99 +1194,99 @@
       <c r="M5" s="1">
         <v>15</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <v>0.57999999999999996</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="2">
         <v>0.12</v>
       </c>
       <c r="P5" s="1">
         <v>22</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <v>4</v>
       </c>
-      <c r="R5" s="5">
+      <c r="R5" s="2">
         <v>0.18</v>
       </c>
       <c r="S5" s="1">
         <v>16.489999999999998</v>
       </c>
-      <c r="T5" s="7">
+      <c r="T5" s="2">
         <v>0.06</v>
       </c>
       <c r="U5" s="1">
         <v>17.239999999999998</v>
       </c>
-      <c r="V5" s="7">
+      <c r="V5" s="2">
         <v>0.03</v>
       </c>
       <c r="W5" s="1">
         <v>18.850000000000001</v>
       </c>
-      <c r="X5" s="5">
+      <c r="X5" s="2">
         <v>0.21</v>
       </c>
       <c r="Y5" s="1">
         <v>17.14</v>
       </c>
-      <c r="Z5" s="5">
+      <c r="Z5" s="2">
         <v>0.19</v>
       </c>
       <c r="AA5" s="1">
         <v>13.95</v>
       </c>
-      <c r="AB5" s="5">
+      <c r="AB5" s="2">
         <v>0.04</v>
       </c>
       <c r="AC5" s="1">
         <v>21.94</v>
       </c>
-      <c r="AD5" s="5">
+      <c r="AD5" s="2">
         <v>0.04</v>
       </c>
       <c r="AE5" s="1">
         <v>0.6</v>
       </c>
-      <c r="AF5" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="AG5" s="3">
+      <c r="AF5" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="AG5" s="1">
         <v>1.1499999999999999</v>
       </c>
-      <c r="AH5" s="7">
+      <c r="AH5" s="2">
         <v>0.01</v>
       </c>
       <c r="AI5" s="1">
         <v>0.61</v>
       </c>
-      <c r="AJ5" s="5">
+      <c r="AJ5" s="2">
         <v>0.26</v>
       </c>
       <c r="AK5" s="1">
         <v>0.62</v>
       </c>
-      <c r="AL5" s="5">
+      <c r="AL5" s="2">
         <v>0.09</v>
       </c>
-      <c r="AM5" s="3">
+      <c r="AM5" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN5" s="7">
+      <c r="AN5" s="2">
         <v>0</v>
       </c>
       <c r="AO5" s="1">
         <v>1.24</v>
       </c>
-      <c r="AP5" s="7">
+      <c r="AP5" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1">
@@ -1304,25 +1295,25 @@
       <c r="D6" s="1">
         <v>0.09</v>
       </c>
-      <c r="E6" s="1">
-        <v>1746</v>
-      </c>
-      <c r="F6" s="1">
-        <v>66</v>
+      <c r="E6" s="7">
+        <v>0.19</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.01</v>
       </c>
       <c r="G6" s="1">
         <v>208</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>34.229999999999997</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>2.79</v>
       </c>
       <c r="J6" s="1">
         <v>130</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <v>59.84</v>
       </c>
       <c r="L6" s="1">
@@ -1331,99 +1322,99 @@
       <c r="M6" s="1">
         <v>15</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <v>1.35</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="2">
         <v>0.06</v>
       </c>
       <c r="P6" s="1">
         <v>21</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <v>4.58</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="2">
         <v>0.27</v>
       </c>
       <c r="S6" s="1">
         <v>16.05</v>
       </c>
-      <c r="T6" s="7">
+      <c r="T6" s="2">
         <v>0.1</v>
       </c>
       <c r="U6" s="1">
         <v>17.399999999999999</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V6" s="2">
         <v>0.03</v>
       </c>
       <c r="W6" s="1">
         <v>19.62</v>
       </c>
-      <c r="X6" s="5">
+      <c r="X6" s="2">
         <v>0.17</v>
       </c>
       <c r="Y6" s="1">
         <v>17.72</v>
       </c>
-      <c r="Z6" s="5">
+      <c r="Z6" s="2">
         <v>0.09</v>
       </c>
       <c r="AA6" s="1">
         <v>14.24</v>
       </c>
-      <c r="AB6" s="5">
+      <c r="AB6" s="2">
         <v>0.03</v>
       </c>
       <c r="AC6" s="1">
         <v>21.97</v>
       </c>
-      <c r="AD6" s="5">
+      <c r="AD6" s="2">
         <v>0.03</v>
       </c>
       <c r="AE6" s="1">
         <v>1.04</v>
       </c>
-      <c r="AF6" s="7">
+      <c r="AF6" s="2">
         <v>0.05</v>
       </c>
-      <c r="AG6" s="3">
+      <c r="AG6" s="1">
         <v>1.4</v>
       </c>
-      <c r="AH6" s="7">
+      <c r="AH6" s="2">
         <v>0.03</v>
       </c>
       <c r="AI6" s="1">
         <v>0.31</v>
       </c>
-      <c r="AJ6" s="5">
+      <c r="AJ6" s="2">
         <v>0.21</v>
       </c>
       <c r="AK6" s="1">
         <v>0.85</v>
       </c>
-      <c r="AL6" s="5">
+      <c r="AL6" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AM6" s="3">
+      <c r="AM6" s="1">
         <v>0.04</v>
       </c>
-      <c r="AN6" s="7">
+      <c r="AN6" s="2">
         <v>0</v>
       </c>
       <c r="AO6" s="1">
         <v>1.75</v>
       </c>
-      <c r="AP6" s="7">
+      <c r="AP6" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1">
@@ -1432,25 +1423,25 @@
       <c r="D7" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E7" s="1">
-        <v>1948</v>
-      </c>
-      <c r="F7" s="1">
-        <v>62</v>
+      <c r="E7" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.02</v>
       </c>
       <c r="G7" s="1">
         <v>196</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>26.03</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>1.88</v>
       </c>
       <c r="J7" s="1">
         <v>155</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>69.55</v>
       </c>
       <c r="L7" s="1">
@@ -1459,99 +1450,99 @@
       <c r="M7" s="1">
         <v>15</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="3">
         <v>0.64</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="2">
         <v>0.11</v>
       </c>
       <c r="P7" s="1">
         <v>19</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <v>3.79</v>
       </c>
-      <c r="R7" s="5">
+      <c r="R7" s="2">
         <v>0.16</v>
       </c>
       <c r="S7" s="1">
         <v>16.39</v>
       </c>
-      <c r="T7" s="7">
+      <c r="T7" s="2">
         <v>0.06</v>
       </c>
       <c r="U7" s="1">
         <v>17.29</v>
       </c>
-      <c r="V7" s="7">
+      <c r="V7" s="2">
         <v>0.03</v>
       </c>
       <c r="W7" s="1">
         <v>17.72</v>
       </c>
-      <c r="X7" s="5">
+      <c r="X7" s="2">
         <v>0.53</v>
       </c>
       <c r="Y7" s="1">
         <v>16.61</v>
       </c>
-      <c r="Z7" s="5">
+      <c r="Z7" s="2">
         <v>0.33</v>
       </c>
       <c r="AA7" s="1">
         <v>13.94</v>
       </c>
-      <c r="AB7" s="5">
+      <c r="AB7" s="2">
         <v>0.04</v>
       </c>
       <c r="AC7" s="1">
         <v>21.96</v>
       </c>
-      <c r="AD7" s="5">
+      <c r="AD7" s="2">
         <v>0.04</v>
       </c>
       <c r="AE7" s="1">
         <v>0.6</v>
       </c>
-      <c r="AF7" s="7">
+      <c r="AF7" s="2">
         <v>0.01</v>
       </c>
-      <c r="AG7" s="3">
+      <c r="AG7" s="1">
         <v>1.2</v>
       </c>
-      <c r="AH7" s="7">
+      <c r="AH7" s="2">
         <v>0.02</v>
       </c>
       <c r="AI7" s="1">
         <v>0.85</v>
       </c>
-      <c r="AJ7" s="5">
+      <c r="AJ7" s="2">
         <v>0.28000000000000003</v>
       </c>
       <c r="AK7" s="1">
         <v>0.94</v>
       </c>
-      <c r="AL7" s="5">
+      <c r="AL7" s="2">
         <v>0.22</v>
       </c>
-      <c r="AM7" s="3">
+      <c r="AM7" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN7" s="7">
+      <c r="AN7" s="2">
         <v>0</v>
       </c>
       <c r="AO7" s="1">
         <v>1.27</v>
       </c>
-      <c r="AP7" s="7">
+      <c r="AP7" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
@@ -1560,25 +1551,25 @@
       <c r="D8" s="1">
         <v>0.08</v>
       </c>
-      <c r="E8" s="1">
-        <v>1855</v>
-      </c>
-      <c r="F8" s="1">
-        <v>77</v>
+      <c r="E8" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.01</v>
       </c>
       <c r="G8" s="1">
         <v>212</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>38.15</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>2.15</v>
       </c>
       <c r="J8" s="1">
         <v>129</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <v>56.02</v>
       </c>
       <c r="L8" s="1">
@@ -1587,99 +1578,99 @@
       <c r="M8" s="1">
         <v>15</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="3">
         <v>1.48</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="2">
         <v>0.04</v>
       </c>
       <c r="P8" s="1">
         <v>21</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <v>4.34</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="2">
         <v>0.25</v>
       </c>
       <c r="S8" s="1">
         <v>16.239999999999998</v>
       </c>
-      <c r="T8" s="7">
+      <c r="T8" s="2">
         <v>0.06</v>
       </c>
       <c r="U8" s="1">
         <v>17.39</v>
       </c>
-      <c r="V8" s="7">
+      <c r="V8" s="2">
         <v>0.02</v>
       </c>
       <c r="W8" s="1">
         <v>19.579999999999998</v>
       </c>
-      <c r="X8" s="5">
+      <c r="X8" s="2">
         <v>0.17</v>
       </c>
       <c r="Y8" s="1">
         <v>17.53</v>
       </c>
-      <c r="Z8" s="5">
+      <c r="Z8" s="2">
         <v>0.1</v>
       </c>
       <c r="AA8" s="1">
         <v>14.19</v>
       </c>
-      <c r="AB8" s="5">
+      <c r="AB8" s="2">
         <v>0.03</v>
       </c>
       <c r="AC8" s="1">
         <v>22.05</v>
       </c>
-      <c r="AD8" s="5">
+      <c r="AD8" s="2">
         <v>0.03</v>
       </c>
       <c r="AE8" s="1">
         <v>0.91</v>
       </c>
-      <c r="AF8" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="AG8" s="3">
+      <c r="AF8" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="AG8" s="1">
         <v>1.39</v>
       </c>
-      <c r="AH8" s="7">
+      <c r="AH8" s="2">
         <v>0.02</v>
       </c>
       <c r="AI8" s="1">
         <v>0.37</v>
       </c>
-      <c r="AJ8" s="5">
+      <c r="AJ8" s="2">
         <v>0.24</v>
       </c>
       <c r="AK8" s="1">
         <v>0.79</v>
       </c>
-      <c r="AL8" s="5">
+      <c r="AL8" s="2">
         <v>0.08</v>
       </c>
-      <c r="AM8" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="AN8" s="7">
+      <c r="AM8" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="AN8" s="2">
         <v>0</v>
       </c>
       <c r="AO8" s="1">
         <v>1.79</v>
       </c>
-      <c r="AP8" s="7">
+      <c r="AP8" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1">
@@ -1688,25 +1679,25 @@
       <c r="D9" s="1">
         <v>0.19</v>
       </c>
-      <c r="E9" s="1">
-        <v>1983</v>
-      </c>
-      <c r="F9" s="1">
-        <v>113</v>
+      <c r="E9" s="7">
+        <v>0.49</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.03</v>
       </c>
       <c r="G9" s="1">
         <v>200</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>27.82</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>2.5</v>
       </c>
       <c r="J9" s="1">
         <v>151</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="3">
         <v>67.81</v>
       </c>
       <c r="L9" s="1">
@@ -1715,99 +1706,99 @@
       <c r="M9" s="1">
         <v>15</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="3">
         <v>0.53</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="2">
         <v>0.13</v>
       </c>
       <c r="P9" s="1">
         <v>19</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <v>3.85</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="2">
         <v>0.24</v>
       </c>
       <c r="S9" s="1">
         <v>16.440000000000001</v>
       </c>
-      <c r="T9" s="7">
+      <c r="T9" s="2">
         <v>0.05</v>
       </c>
       <c r="U9" s="1">
         <v>17.28</v>
       </c>
-      <c r="V9" s="7">
+      <c r="V9" s="2">
         <v>0.04</v>
       </c>
       <c r="W9" s="1">
         <v>18.73</v>
       </c>
-      <c r="X9" s="5">
+      <c r="X9" s="2">
         <v>0.24</v>
       </c>
       <c r="Y9" s="1">
         <v>17.28</v>
       </c>
-      <c r="Z9" s="5">
+      <c r="Z9" s="2">
         <v>0.2</v>
       </c>
       <c r="AA9" s="1">
         <v>13.98</v>
       </c>
-      <c r="AB9" s="5">
+      <c r="AB9" s="2">
         <v>0.04</v>
       </c>
       <c r="AC9" s="1">
         <v>21.92</v>
       </c>
-      <c r="AD9" s="5">
+      <c r="AD9" s="2">
         <v>0.04</v>
       </c>
       <c r="AE9" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AF9" s="7">
+      <c r="AF9" s="2">
         <v>0.01</v>
       </c>
-      <c r="AG9" s="3">
+      <c r="AG9" s="1">
         <v>1.2</v>
       </c>
-      <c r="AH9" s="7">
+      <c r="AH9" s="2">
         <v>0.01</v>
       </c>
       <c r="AI9" s="1">
         <v>0.87</v>
       </c>
-      <c r="AJ9" s="5">
+      <c r="AJ9" s="2">
         <v>0.34</v>
       </c>
       <c r="AK9" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AL9" s="5">
+      <c r="AL9" s="2">
         <v>0.11</v>
       </c>
-      <c r="AM9" s="3">
+      <c r="AM9" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN9" s="7">
+      <c r="AN9" s="2">
         <v>0</v>
       </c>
       <c r="AO9" s="1">
         <v>1.24</v>
       </c>
-      <c r="AP9" s="7">
+      <c r="AP9" s="2">
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1">
@@ -1816,25 +1807,25 @@
       <c r="D10" s="1">
         <v>0.09</v>
       </c>
-      <c r="E10" s="1">
-        <v>1818</v>
-      </c>
-      <c r="F10" s="1">
-        <v>52</v>
+      <c r="E10" s="7">
+        <v>0.19</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.01</v>
       </c>
       <c r="G10" s="1">
         <v>213</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>36.479999999999997</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>2.67</v>
       </c>
       <c r="J10" s="1">
         <v>126</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <v>57.64</v>
       </c>
       <c r="L10" s="1">
@@ -1843,99 +1834,99 @@
       <c r="M10" s="1">
         <v>15</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="3">
         <v>1.62</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="P10" s="1">
         <v>22</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <v>4.2699999999999996</v>
       </c>
-      <c r="R10" s="5">
+      <c r="R10" s="2">
         <v>0.19</v>
       </c>
       <c r="S10" s="1">
         <v>16.3</v>
       </c>
-      <c r="T10" s="7">
+      <c r="T10" s="2">
         <v>0.08</v>
       </c>
       <c r="U10" s="1">
         <v>17.350000000000001</v>
       </c>
-      <c r="V10" s="7">
+      <c r="V10" s="2">
         <v>0.02</v>
       </c>
       <c r="W10" s="1">
         <v>18.54</v>
       </c>
-      <c r="X10" s="5">
+      <c r="X10" s="2">
         <v>0.43</v>
       </c>
       <c r="Y10" s="1">
         <v>16.95</v>
       </c>
-      <c r="Z10" s="5">
+      <c r="Z10" s="2">
         <v>0.23</v>
       </c>
       <c r="AA10" s="1">
         <v>14.23</v>
       </c>
-      <c r="AB10" s="5">
+      <c r="AB10" s="2">
         <v>0.04</v>
       </c>
       <c r="AC10" s="1">
         <v>21.99</v>
       </c>
-      <c r="AD10" s="5">
+      <c r="AD10" s="2">
         <v>0.03</v>
       </c>
       <c r="AE10" s="1">
         <v>0.81</v>
       </c>
-      <c r="AF10" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="AG10" s="3">
+      <c r="AF10" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="AG10" s="1">
         <v>1.36</v>
       </c>
-      <c r="AH10" s="7">
+      <c r="AH10" s="2">
         <v>0.02</v>
       </c>
       <c r="AI10" s="1">
         <v>0.44</v>
       </c>
-      <c r="AJ10" s="5">
+      <c r="AJ10" s="2">
         <v>0.17</v>
       </c>
       <c r="AK10" s="1">
         <v>1.05</v>
       </c>
-      <c r="AL10" s="5">
+      <c r="AL10" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AM10" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="AN10" s="7">
+      <c r="AM10" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="AN10" s="2">
         <v>0</v>
       </c>
       <c r="AO10" s="1">
         <v>1.76</v>
       </c>
-      <c r="AP10" s="7">
+      <c r="AP10" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1">
@@ -1944,25 +1935,25 @@
       <c r="D11" s="1">
         <v>0.12</v>
       </c>
-      <c r="E11" s="1">
-        <v>2155</v>
-      </c>
-      <c r="F11" s="1">
-        <v>119</v>
+      <c r="E11" s="7">
+        <v>0.47</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.03</v>
       </c>
       <c r="G11" s="1">
         <v>196</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>30.05</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>2.04</v>
       </c>
       <c r="J11" s="1">
         <v>148</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <v>65.900000000000006</v>
       </c>
       <c r="L11" s="1">
@@ -1971,99 +1962,99 @@
       <c r="M11" s="1">
         <v>15</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="3">
         <v>0.61</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="2">
         <v>0.13</v>
       </c>
       <c r="P11" s="1">
         <v>19</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <v>3.45</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="2">
         <v>0.18</v>
       </c>
       <c r="S11" s="1">
         <v>16.489999999999998</v>
       </c>
-      <c r="T11" s="7">
+      <c r="T11" s="2">
         <v>0.06</v>
       </c>
       <c r="U11" s="1">
         <v>17.23</v>
       </c>
-      <c r="V11" s="7">
+      <c r="V11" s="2">
         <v>0.03</v>
       </c>
       <c r="W11" s="1">
         <v>18.84</v>
       </c>
-      <c r="X11" s="5">
+      <c r="X11" s="2">
         <v>0.24</v>
       </c>
       <c r="Y11" s="1">
         <v>17.239999999999998</v>
       </c>
-      <c r="Z11" s="5">
+      <c r="Z11" s="2">
         <v>0.15</v>
       </c>
       <c r="AA11" s="1">
         <v>13.99</v>
       </c>
-      <c r="AB11" s="5">
+      <c r="AB11" s="2">
         <v>0.03</v>
       </c>
       <c r="AC11" s="1">
         <v>21.94</v>
       </c>
-      <c r="AD11" s="5">
+      <c r="AD11" s="2">
         <v>0.03</v>
       </c>
       <c r="AE11" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AF11" s="7">
+      <c r="AF11" s="2">
         <v>0.01</v>
       </c>
-      <c r="AG11" s="3">
+      <c r="AG11" s="1">
         <v>1.18</v>
       </c>
-      <c r="AH11" s="7">
+      <c r="AH11" s="2">
         <v>0.01</v>
       </c>
       <c r="AI11" s="1">
         <v>0.71</v>
       </c>
-      <c r="AJ11" s="5">
+      <c r="AJ11" s="2">
         <v>0.32</v>
       </c>
       <c r="AK11" s="1">
         <v>0.61</v>
       </c>
-      <c r="AL11" s="5">
+      <c r="AL11" s="2">
         <v>0.1</v>
       </c>
-      <c r="AM11" s="3">
+      <c r="AM11" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN11" s="7">
+      <c r="AN11" s="2">
         <v>0</v>
       </c>
       <c r="AO11" s="1">
         <v>1.28</v>
       </c>
-      <c r="AP11" s="7">
+      <c r="AP11" s="2">
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1">
@@ -2072,25 +2063,25 @@
       <c r="D12" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E12" s="1">
-        <v>1774</v>
-      </c>
-      <c r="F12" s="1">
-        <v>121</v>
+      <c r="E12" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.01</v>
       </c>
       <c r="G12" s="1">
         <v>206</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>33.46</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>3.48</v>
       </c>
       <c r="J12" s="1">
         <v>126</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="3">
         <v>60.19</v>
       </c>
       <c r="L12" s="1">
@@ -2099,99 +2090,99 @@
       <c r="M12" s="1">
         <v>16</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="3">
         <v>1.41</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="2">
         <v>0.06</v>
       </c>
       <c r="P12" s="1">
         <v>21</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12" s="3">
         <v>4.9400000000000004</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R12" s="2">
         <v>0.42</v>
       </c>
       <c r="S12" s="1">
         <v>16.260000000000002</v>
       </c>
-      <c r="T12" s="7">
+      <c r="T12" s="2">
         <v>0.08</v>
       </c>
       <c r="U12" s="1">
         <v>17.420000000000002</v>
       </c>
-      <c r="V12" s="7">
+      <c r="V12" s="2">
         <v>0.03</v>
       </c>
       <c r="W12" s="1">
         <v>19.64</v>
       </c>
-      <c r="X12" s="5">
+      <c r="X12" s="2">
         <v>0.21</v>
       </c>
       <c r="Y12" s="1">
         <v>17.32</v>
       </c>
-      <c r="Z12" s="5">
+      <c r="Z12" s="2">
         <v>0.11</v>
       </c>
       <c r="AA12" s="1">
         <v>14.27</v>
       </c>
-      <c r="AB12" s="5">
+      <c r="AB12" s="2">
         <v>0.05</v>
       </c>
       <c r="AC12" s="1">
         <v>21.95</v>
       </c>
-      <c r="AD12" s="5">
+      <c r="AD12" s="2">
         <v>0.04</v>
       </c>
       <c r="AE12" s="1">
         <v>0.97</v>
       </c>
-      <c r="AF12" s="7">
+      <c r="AF12" s="2">
         <v>0.04</v>
       </c>
-      <c r="AG12" s="3">
+      <c r="AG12" s="1">
         <v>1.42</v>
       </c>
-      <c r="AH12" s="7">
+      <c r="AH12" s="2">
         <v>0.03</v>
       </c>
       <c r="AI12" s="1">
         <v>0.2</v>
       </c>
-      <c r="AJ12" s="5">
+      <c r="AJ12" s="2">
         <v>0.19</v>
       </c>
       <c r="AK12" s="1">
         <v>0.8</v>
       </c>
-      <c r="AL12" s="5">
+      <c r="AL12" s="2">
         <v>0.08</v>
       </c>
-      <c r="AM12" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="AN12" s="7">
+      <c r="AM12" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="AN12" s="2">
         <v>0</v>
       </c>
       <c r="AO12" s="1">
         <v>1.79</v>
       </c>
-      <c r="AP12" s="7">
+      <c r="AP12" s="2">
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1">
@@ -2200,25 +2191,25 @@
       <c r="D13" s="1">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E13" s="1">
-        <v>2037</v>
-      </c>
-      <c r="F13" s="1">
-        <v>156</v>
+      <c r="E13" s="7">
+        <v>0.41</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.05</v>
       </c>
       <c r="G13" s="1">
         <v>197</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <v>26.3</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <v>3.55</v>
       </c>
       <c r="J13" s="1">
         <v>149</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="3">
         <v>69.02</v>
       </c>
       <c r="L13" s="1">
@@ -2227,99 +2218,99 @@
       <c r="M13" s="1">
         <v>16</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="3">
         <v>0.57999999999999996</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="2">
         <v>0.21</v>
       </c>
       <c r="P13" s="1">
         <v>20</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="Q13" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="R13" s="5">
+      <c r="R13" s="2">
         <v>0.46</v>
       </c>
       <c r="S13" s="1">
         <v>16.45</v>
       </c>
-      <c r="T13" s="7">
+      <c r="T13" s="2">
         <v>0.11</v>
       </c>
       <c r="U13" s="1">
         <v>17.28</v>
       </c>
-      <c r="V13" s="7">
+      <c r="V13" s="2">
         <v>0.05</v>
       </c>
       <c r="W13" s="1">
         <v>18.61</v>
       </c>
-      <c r="X13" s="5">
+      <c r="X13" s="2">
         <v>0.25</v>
       </c>
       <c r="Y13" s="1">
         <v>17.38</v>
       </c>
-      <c r="Z13" s="5">
+      <c r="Z13" s="2">
         <v>0.21</v>
       </c>
       <c r="AA13" s="1">
         <v>13.99</v>
       </c>
-      <c r="AB13" s="5">
+      <c r="AB13" s="2">
         <v>0.08</v>
       </c>
       <c r="AC13" s="1">
         <v>21.94</v>
       </c>
-      <c r="AD13" s="5">
+      <c r="AD13" s="2">
         <v>0.1</v>
       </c>
       <c r="AE13" s="1">
         <v>0.61</v>
       </c>
-      <c r="AF13" s="7">
+      <c r="AF13" s="2">
         <v>0.04</v>
       </c>
-      <c r="AG13" s="3">
+      <c r="AG13" s="1">
         <v>1.24</v>
       </c>
-      <c r="AH13" s="7">
+      <c r="AH13" s="2">
         <v>0.02</v>
       </c>
       <c r="AI13" s="1">
         <v>0.9</v>
       </c>
-      <c r="AJ13" s="5">
+      <c r="AJ13" s="2">
         <v>0.35</v>
       </c>
       <c r="AK13" s="1">
         <v>0.5</v>
       </c>
-      <c r="AL13" s="5">
+      <c r="AL13" s="2">
         <v>0.08</v>
       </c>
-      <c r="AM13" s="3">
+      <c r="AM13" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN13" s="7">
+      <c r="AN13" s="2">
         <v>0.01</v>
       </c>
       <c r="AO13" s="1">
         <v>1.34</v>
       </c>
-      <c r="AP13" s="7">
+      <c r="AP13" s="2">
         <v>0.04</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1">
@@ -2328,25 +2319,25 @@
       <c r="D14" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E14" s="1">
-        <v>1970</v>
-      </c>
-      <c r="F14" s="1">
-        <v>56</v>
+      <c r="E14" s="7">
+        <v>0.17</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.01</v>
       </c>
       <c r="G14" s="1">
         <v>207</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <v>43.09</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <v>1.2</v>
       </c>
       <c r="J14" s="1">
         <v>130</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="3">
         <v>51.44</v>
       </c>
       <c r="L14" s="1">
@@ -2355,99 +2346,99 @@
       <c r="M14" s="1">
         <v>16</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14" s="3">
         <v>1.48</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="2">
         <v>0.05</v>
       </c>
       <c r="P14" s="1">
         <v>20</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="Q14" s="3">
         <v>3.99</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="2">
         <v>0.11</v>
       </c>
       <c r="S14" s="1">
         <v>16.13</v>
       </c>
-      <c r="T14" s="7">
+      <c r="T14" s="2">
         <v>0.06</v>
       </c>
       <c r="U14" s="1">
         <v>17.39</v>
       </c>
-      <c r="V14" s="7">
+      <c r="V14" s="2">
         <v>0.02</v>
       </c>
       <c r="W14" s="1">
         <v>19.59</v>
       </c>
-      <c r="X14" s="5">
+      <c r="X14" s="2">
         <v>0.15</v>
       </c>
       <c r="Y14" s="1">
         <v>17.579999999999998</v>
       </c>
-      <c r="Z14" s="5">
+      <c r="Z14" s="2">
         <v>0.1</v>
       </c>
       <c r="AA14" s="1">
         <v>14.23</v>
       </c>
-      <c r="AB14" s="5">
+      <c r="AB14" s="2">
         <v>0.03</v>
       </c>
       <c r="AC14" s="1">
         <v>21.99</v>
       </c>
-      <c r="AD14" s="5">
+      <c r="AD14" s="2">
         <v>0.03</v>
       </c>
       <c r="AE14" s="1">
         <v>0.88</v>
       </c>
-      <c r="AF14" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="AG14" s="3">
+      <c r="AF14" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="AG14" s="1">
         <v>1.37</v>
       </c>
-      <c r="AH14" s="7">
+      <c r="AH14" s="2">
         <v>0.02</v>
       </c>
       <c r="AI14" s="1">
         <v>0.35</v>
       </c>
-      <c r="AJ14" s="5">
+      <c r="AJ14" s="2">
         <v>0.16</v>
       </c>
       <c r="AK14" s="1">
         <v>0.88</v>
       </c>
-      <c r="AL14" s="5">
+      <c r="AL14" s="2">
         <v>0.06</v>
       </c>
-      <c r="AM14" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="AN14" s="7">
+      <c r="AM14" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="AN14" s="2">
         <v>0</v>
       </c>
       <c r="AO14" s="1">
         <v>1.75</v>
       </c>
-      <c r="AP14" s="7">
+      <c r="AP14" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="1">
@@ -2456,25 +2447,25 @@
       <c r="D15" s="1">
         <v>0.3</v>
       </c>
-      <c r="E15" s="1">
-        <v>1800</v>
-      </c>
-      <c r="F15" s="1">
-        <v>103</v>
+      <c r="E15" s="7">
+        <v>0.38</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0.03</v>
       </c>
       <c r="G15" s="1">
         <v>196</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>21.41</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>3.16</v>
       </c>
       <c r="J15" s="1">
         <v>149</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="3">
         <v>73.819999999999993</v>
       </c>
       <c r="L15" s="1">
@@ -2483,97 +2474,97 @@
       <c r="M15" s="1">
         <v>16</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15" s="3">
         <v>0.48</v>
       </c>
-      <c r="O15" s="5">
+      <c r="O15" s="2">
         <v>0.12</v>
       </c>
       <c r="P15" s="1">
         <v>21</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="Q15" s="3">
         <v>4.29</v>
       </c>
-      <c r="R15" s="5">
+      <c r="R15" s="2">
         <v>0.28000000000000003</v>
       </c>
       <c r="S15" s="1">
         <v>16.420000000000002</v>
       </c>
-      <c r="T15" s="7">
+      <c r="T15" s="2">
         <v>0.08</v>
       </c>
       <c r="U15" s="1">
         <v>17.27</v>
       </c>
-      <c r="V15" s="7">
+      <c r="V15" s="2">
         <v>0.03</v>
       </c>
       <c r="W15" s="1">
         <v>19.05</v>
       </c>
-      <c r="X15" s="5">
+      <c r="X15" s="2">
         <v>0.23</v>
       </c>
       <c r="Y15" s="1">
         <v>17.16</v>
       </c>
-      <c r="Z15" s="5">
+      <c r="Z15" s="2">
         <v>0.21</v>
       </c>
       <c r="AA15" s="1">
         <v>14.03</v>
       </c>
-      <c r="AB15" s="5">
+      <c r="AB15" s="2">
         <v>0.05</v>
       </c>
       <c r="AC15" s="1">
         <v>21.91</v>
       </c>
-      <c r="AD15" s="5">
+      <c r="AD15" s="2">
         <v>0.05</v>
       </c>
       <c r="AE15" s="1">
         <v>0.61</v>
       </c>
-      <c r="AF15" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="AG15" s="8">
+      <c r="AF15" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="AG15" s="4">
         <v>1.23</v>
       </c>
-      <c r="AH15" s="7">
+      <c r="AH15" s="2">
         <v>0.02</v>
       </c>
       <c r="AI15" s="1">
         <v>0.33</v>
       </c>
-      <c r="AJ15" s="5">
+      <c r="AJ15" s="2">
         <v>0.18</v>
       </c>
       <c r="AK15" s="1">
         <v>0.69</v>
       </c>
-      <c r="AL15" s="5">
+      <c r="AL15" s="2">
         <v>0.08</v>
       </c>
       <c r="AM15" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN15" s="7">
+      <c r="AN15" s="2">
         <v>0</v>
       </c>
       <c r="AO15" s="1">
         <v>1.32</v>
       </c>
-      <c r="AP15" s="7">
+      <c r="AP15" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Edited Figure 1 and S1
</commit_message>
<xml_diff>
--- a/data/Data_F1.xlsx
+++ b/data/Data_F1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/pra100_csiro_au/Documents/Documents/Lipids_manuscript02/Qfly_domestication/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="8_{A1D12656-BE65-4D83-8667-FBA7005B926B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9FAE138-471A-4F8C-A7C1-4A291431DD12}"/>
+  <xr:revisionPtr revIDLastSave="212" documentId="8_{A1D12656-BE65-4D83-8667-FBA7005B926B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02D26BB7-F2D8-4A58-BC82-D407F37F34C2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E200BEC2-E4DD-47C8-9E02-F4549D1DECE6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t xml:space="preserve">CTnew       </t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>ELPLs.AcylDB.SE</t>
+  </si>
+  <si>
+    <t>Pt</t>
+  </si>
+  <si>
+    <t>Pt.Se</t>
   </si>
 </sst>
 </file>
@@ -239,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,9 +265,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -277,6 +280,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -596,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3582FE2B-FBA7-477D-9390-AEEE4D7CC41D}">
-  <dimension ref="A1:AP16"/>
+  <dimension ref="A1:AR16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,7 +649,7 @@
     <col min="42" max="42" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
@@ -769,8 +776,14 @@
       <c r="AP1" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="AQ1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -783,10 +796,10 @@
       <c r="D2" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="1">
         <v>0.19</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="1">
         <v>0.01</v>
       </c>
       <c r="G2" s="1">
@@ -897,8 +910,14 @@
       <c r="AP2" s="2">
         <v>0.02</v>
       </c>
+      <c r="AQ2" s="2">
+        <v>8.91</v>
+      </c>
+      <c r="AR2" s="2">
+        <v>0.33</v>
+      </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -911,10 +930,10 @@
       <c r="D3" s="1">
         <v>0.33</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="1">
         <v>0.42</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="1">
         <v>0.02</v>
       </c>
       <c r="G3" s="1">
@@ -1025,8 +1044,14 @@
       <c r="AP3" s="2">
         <v>0.03</v>
       </c>
+      <c r="AQ3" s="2">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="AR3" s="2">
+        <v>0.44</v>
+      </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1039,10 +1064,10 @@
       <c r="D4" s="1">
         <v>0.1</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="1">
         <v>0.13</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="1">
         <v>0.01</v>
       </c>
       <c r="G4" s="1">
@@ -1153,8 +1178,14 @@
       <c r="AP4" s="2">
         <v>0.02</v>
       </c>
+      <c r="AQ4" s="2">
+        <v>7.72</v>
+      </c>
+      <c r="AR4" s="2">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1167,10 +1198,10 @@
       <c r="D5" s="1">
         <v>0.23</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="1">
         <v>0.42</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="1">
         <v>0.02</v>
       </c>
       <c r="G5" s="1">
@@ -1281,8 +1312,14 @@
       <c r="AP5" s="2">
         <v>0.02</v>
       </c>
+      <c r="AQ5" s="2">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="AR5" s="2">
+        <v>0.39</v>
+      </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1295,10 +1332,10 @@
       <c r="D6" s="1">
         <v>0.09</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="1">
         <v>0.19</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="1">
         <v>0.01</v>
       </c>
       <c r="G6" s="1">
@@ -1409,8 +1446,14 @@
       <c r="AP6" s="2">
         <v>0.02</v>
       </c>
+      <c r="AQ6" s="2">
+        <v>8.73</v>
+      </c>
+      <c r="AR6" s="2">
+        <v>0.33</v>
+      </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
@@ -1423,10 +1466,10 @@
       <c r="D7" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="1">
         <v>0.45</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="1">
         <v>0.02</v>
       </c>
       <c r="G7" s="1">
@@ -1537,8 +1580,14 @@
       <c r="AP7" s="2">
         <v>0.02</v>
       </c>
+      <c r="AQ7" s="2">
+        <v>9.74</v>
+      </c>
+      <c r="AR7" s="2">
+        <v>0.31</v>
+      </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1551,10 +1600,10 @@
       <c r="D8" s="1">
         <v>0.08</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="1">
         <v>0.18</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="1">
         <v>0.01</v>
       </c>
       <c r="G8" s="1">
@@ -1665,8 +1714,14 @@
       <c r="AP8" s="2">
         <v>0.02</v>
       </c>
+      <c r="AQ8" s="2">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="AR8" s="2">
+        <v>0.32</v>
+      </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
@@ -1679,10 +1734,10 @@
       <c r="D9" s="1">
         <v>0.19</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="1">
         <v>0.49</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="1">
         <v>0.03</v>
       </c>
       <c r="G9" s="1">
@@ -1793,8 +1848,14 @@
       <c r="AP9" s="2">
         <v>0.01</v>
       </c>
+      <c r="AQ9" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="AR9" s="2">
+        <v>0.55000000000000004</v>
+      </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -1807,10 +1868,10 @@
       <c r="D10" s="1">
         <v>0.09</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="1">
         <v>0.19</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="1">
         <v>0.01</v>
       </c>
       <c r="G10" s="1">
@@ -1921,8 +1982,14 @@
       <c r="AP10" s="2">
         <v>0.02</v>
       </c>
+      <c r="AQ10" s="2">
+        <v>9.09</v>
+      </c>
+      <c r="AR10" s="2">
+        <v>0.26</v>
+      </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1935,10 +2002,10 @@
       <c r="D11" s="1">
         <v>0.12</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="1">
         <v>0.47</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="1">
         <v>0.03</v>
       </c>
       <c r="G11" s="1">
@@ -2049,8 +2116,14 @@
       <c r="AP11" s="2">
         <v>0.01</v>
       </c>
+      <c r="AQ11" s="2">
+        <v>10.8</v>
+      </c>
+      <c r="AR11" s="2">
+        <v>0.59</v>
+      </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>5</v>
       </c>
@@ -2063,10 +2136,10 @@
       <c r="D12" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="1">
         <v>0.18</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="1">
         <v>0.01</v>
       </c>
       <c r="G12" s="1">
@@ -2177,8 +2250,14 @@
       <c r="AP12" s="2">
         <v>0.03</v>
       </c>
+      <c r="AQ12" s="2">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="AR12" s="2">
+        <v>0.6</v>
+      </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>5</v>
       </c>
@@ -2191,10 +2270,10 @@
       <c r="D13" s="1">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="1">
         <v>0.41</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="1">
         <v>0.05</v>
       </c>
       <c r="G13" s="1">
@@ -2305,8 +2384,14 @@
       <c r="AP13" s="2">
         <v>0.04</v>
       </c>
+      <c r="AQ13" s="2">
+        <v>9.89</v>
+      </c>
+      <c r="AR13" s="2">
+        <v>1.1200000000000001</v>
+      </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
@@ -2319,10 +2404,10 @@
       <c r="D14" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="1">
         <v>0.17</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="1">
         <v>0.01</v>
       </c>
       <c r="G14" s="1">
@@ -2433,8 +2518,14 @@
       <c r="AP14" s="2">
         <v>0.02</v>
       </c>
+      <c r="AQ14" s="2">
+        <v>9.85</v>
+      </c>
+      <c r="AR14" s="2">
+        <v>0.28000000000000003</v>
+      </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
@@ -2447,10 +2538,10 @@
       <c r="D15" s="1">
         <v>0.3</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="1">
         <v>0.38</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="1">
         <v>0.03</v>
       </c>
       <c r="G15" s="1">
@@ -2561,8 +2652,14 @@
       <c r="AP15" s="2">
         <v>0.02</v>
       </c>
+      <c r="AQ15" s="2">
+        <v>9</v>
+      </c>
+      <c r="AR15" s="2">
+        <v>0.52</v>
+      </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>

</xml_diff>